<commit_message>
Solicitud gráfica de rec200 ma_11_06
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado11/guion06/SolicitudGrafica MA_11_06_REC200_CO.xlsx
+++ b/fuentes/contenidos/grado11/guion06/SolicitudGrafica MA_11_06_REC200_CO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27224"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joan/Dropbox/Aula planeta/Entregas/Entrega 25 (cuenta para agosto) X/REC200 (M101A)/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lzambrano\Documents\GitHub\Matematicas\fuentes\contenidos\grado11\guion06\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="hX79YNGfHMUCcosWMoH0GQuhNo2gkebFrfW3do2TOcvwqaujU9m0uwOL5UkRtWEspAy/ISD2JB8+jf057W9mVA==" workbookSaltValue="uRz/CDpmZ5ecKheoN1C0Jw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="16240" windowHeight="15940" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="16245" windowHeight="15945" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Solicitud gráfica" sheetId="1" r:id="rId1"/>
@@ -21,11 +21,8 @@
     <definedName name="Formato">'Solicitud gráfica'!$L$2:$L$3</definedName>
     <definedName name="Ubicación">'Solicitud gráfica'!$M$2:$M$6</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -1581,6 +1578,7 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1679,7 +1677,6 @@
     <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="51">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -1786,7 +1783,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="16" dropStyle="combo" dx="33" fmlaLink="$K$44" fmlaRange="$K$4:$K$43" noThreeD="1" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="16" dropStyle="combo" dx="33" fmlaLink="$K$44" fmlaRange="$K$4:$K$43" noThreeD="1" sel="1" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1805,16 +1802,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>169333</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>129647</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>169333</xdr:rowOff>
+      <xdr:rowOff>58208</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>355600</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>2189760</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>1579033</xdr:rowOff>
+      <xdr:rowOff>793750</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1831,8 +1828,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16520583" y="2254250"/>
-          <a:ext cx="9055100" cy="1409700"/>
+          <a:off x="13813897" y="2177521"/>
+          <a:ext cx="4719176" cy="735542"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1843,16 +1840,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>423333</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1558396</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>624417</xdr:rowOff>
+      <xdr:rowOff>418042</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>2190749</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>2034117</xdr:rowOff>
+      <xdr:rowOff>1174770</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1869,8 +1866,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16774583" y="4476750"/>
-          <a:ext cx="9055100" cy="1409700"/>
+          <a:off x="13678959" y="4299480"/>
+          <a:ext cx="4855103" cy="756728"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1881,16 +1878,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>359833</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>304272</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>783166</xdr:rowOff>
+      <xdr:rowOff>219603</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>546100</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>2087563</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>1862666</xdr:rowOff>
+      <xdr:rowOff>749816</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1907,8 +1904,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16711083" y="7291916"/>
-          <a:ext cx="9055100" cy="1079500"/>
+          <a:off x="13988522" y="6752166"/>
+          <a:ext cx="4442354" cy="530213"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1919,16 +1916,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>158750</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>277626</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>603250</xdr:rowOff>
+      <xdr:rowOff>126999</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>345017</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>19579</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>1682750</xdr:rowOff>
+      <xdr:rowOff>682624</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1945,8 +1942,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16510000" y="9958917"/>
-          <a:ext cx="9055100" cy="1079500"/>
+          <a:off x="13961876" y="9501187"/>
+          <a:ext cx="4655266" cy="555625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1965,13 +1962,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>25400</xdr:colOff>
+          <xdr:colOff>28575</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>1041400</xdr:colOff>
+          <xdr:colOff>1038225</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>228600</xdr:rowOff>
         </xdr:to>
@@ -2020,13 +2017,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>1054100</xdr:colOff>
+          <xdr:colOff>1057275</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>863600</xdr:colOff>
+          <xdr:colOff>866775</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>228600</xdr:rowOff>
         </xdr:to>
@@ -2075,7 +2072,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>12700</xdr:colOff>
+          <xdr:colOff>9525</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
@@ -2132,13 +2129,13 @@
           <xdr:col>2</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>482600</xdr:rowOff>
+          <xdr:rowOff>485775</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>1016000</xdr:colOff>
+          <xdr:colOff>1019175</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>711200</xdr:rowOff>
+          <xdr:rowOff>714375</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2185,15 +2182,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>1016000</xdr:colOff>
+          <xdr:colOff>1019175</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>482600</xdr:rowOff>
+          <xdr:rowOff>485775</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
           <xdr:colOff>838200</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>711200</xdr:rowOff>
+          <xdr:rowOff>714375</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2242,13 +2239,13 @@
           <xdr:col>4</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>482600</xdr:rowOff>
+          <xdr:rowOff>485775</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
           <xdr:colOff>838200</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>711200</xdr:rowOff>
+          <xdr:rowOff>714375</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2297,13 +2294,13 @@
           <xdr:col>5</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>482600</xdr:rowOff>
+          <xdr:rowOff>485775</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>5</xdr:col>
           <xdr:colOff>838200</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>711200</xdr:rowOff>
+          <xdr:rowOff>714375</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2670,34 +2667,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Hoja1" enableFormatConditionsCalculation="0"/>
+  <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:P108"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K18" sqref="K18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" style="2" customWidth="1"/>
     <col min="2" max="2" width="21" style="2" customWidth="1"/>
-    <col min="3" max="3" width="21.1640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="21.125" style="2" customWidth="1"/>
     <col min="4" max="4" width="15.5" style="2" customWidth="1"/>
-    <col min="5" max="5" width="17.1640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="28.1640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="17.125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="28.125" style="2" customWidth="1"/>
     <col min="7" max="7" width="20.5" style="2" customWidth="1"/>
-    <col min="8" max="8" width="28.6640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="28.625" style="2" customWidth="1"/>
     <col min="9" max="9" width="20.5" style="2" customWidth="1"/>
-    <col min="10" max="10" width="34.83203125" style="15" customWidth="1"/>
-    <col min="11" max="11" width="29.6640625" style="15" customWidth="1"/>
-    <col min="12" max="12" width="20.33203125" style="2" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="34.875" style="15" customWidth="1"/>
+    <col min="11" max="11" width="29.625" style="15" customWidth="1"/>
+    <col min="12" max="12" width="20.375" style="2" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="14.5" style="2" hidden="1" customWidth="1"/>
-    <col min="14" max="15" width="10.83203125" style="2" hidden="1" customWidth="1"/>
-    <col min="16" max="16384" width="10.83203125" style="2"/>
+    <col min="14" max="15" width="10.875" style="2" hidden="1" customWidth="1"/>
+    <col min="16" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="16.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2716,19 +2713,19 @@
         <v>Ubicación de la imagen en el recurso M101</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C2" s="85" t="s">
+      <c r="C2" s="86" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="86"/>
-      <c r="F2" s="78" t="s">
+      <c r="D2" s="87"/>
+      <c r="F2" s="79" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="79"/>
+      <c r="G2" s="80"/>
       <c r="H2" s="58"/>
       <c r="I2" s="58"/>
       <c r="J2" s="14"/>
@@ -2747,17 +2744,17 @@
         <v>M3A</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="87">
+      <c r="C3" s="88">
         <v>11</v>
       </c>
-      <c r="D3" s="88"/>
-      <c r="F3" s="80"/>
-      <c r="G3" s="81"/>
+      <c r="D3" s="89"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="82"/>
       <c r="H3" s="58"/>
       <c r="I3" s="38"/>
       <c r="J3" s="14"/>
@@ -2776,15 +2773,15 @@
         <v>M5A</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="87" t="s">
+      <c r="C4" s="88" t="s">
         <v>188</v>
       </c>
-      <c r="D4" s="88"/>
+      <c r="D4" s="89"/>
       <c r="E4" s="5"/>
       <c r="F4" s="37" t="s">
         <v>55</v>
@@ -2808,13 +2805,13 @@
         <v>M6A</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="16.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="89"/>
-      <c r="D5" s="90"/>
+      <c r="C5" s="90"/>
+      <c r="D5" s="91"/>
       <c r="E5" s="5"/>
       <c r="F5" s="37" t="str">
         <f>IF(G4="Recurso","Motor del recurso","")</f>
@@ -2839,7 +2836,7 @@
         <v>M7A</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="16.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -2863,7 +2860,7 @@
         <v>M8A</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="24" t="s">
         <v>40</v>
@@ -2892,18 +2889,18 @@
         <v>M9B</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="8" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" s="8" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
-      <c r="F8" s="82" t="s">
+      <c r="F8" s="83" t="s">
         <v>62</v>
       </c>
-      <c r="G8" s="83"/>
-      <c r="H8" s="83"/>
-      <c r="I8" s="84"/>
+      <c r="G8" s="84"/>
+      <c r="H8" s="84"/>
+      <c r="I8" s="85"/>
       <c r="J8" s="16"/>
       <c r="K8" s="11"/>
       <c r="M8" s="2" t="str">
@@ -2919,7 +2916,7 @@
       </c>
       <c r="P8" s="2"/>
     </row>
-    <row r="9" spans="1:16" ht="38.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" ht="38.85" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="21" t="s">
         <v>2</v>
       </c>
@@ -2959,12 +2956,12 @@
         <v>M10B</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="11" customFormat="1" ht="139" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" s="11" customFormat="1" ht="138.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="str">
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),"IMG01","")</f>
         <v>IMG01</v>
       </c>
-      <c r="B10" s="109" t="s">
+      <c r="B10" s="78" t="s">
         <v>189</v>
       </c>
       <c r="C10" s="20" t="str">
@@ -2993,7 +2990,7 @@
         <f ca="1">IF(OR($B10&lt;&gt;"",$J10&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E10,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E10,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>500 x 500 px</v>
       </c>
-      <c r="J10" s="109" t="s">
+      <c r="J10" s="78" t="s">
         <v>191</v>
       </c>
       <c r="K10" s="64"/>
@@ -3002,12 +2999,12 @@
         <v>M12D</v>
       </c>
     </row>
-    <row r="11" spans="1:16" s="11" customFormat="1" ht="209" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" s="11" customFormat="1" ht="209.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="str">
         <f t="shared" ref="A11:A18" si="3">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE(LEFT(A10,3),IF(MID(A10,4,2)+1&lt;10,CONCATENATE("0",MID(A10,4,2)+1))),"")</f>
         <v>IMG02</v>
       </c>
-      <c r="B11" s="109" t="s">
+      <c r="B11" s="78" t="s">
         <v>189</v>
       </c>
       <c r="C11" s="20" t="str">
@@ -3036,7 +3033,7 @@
         <f ca="1">IF(OR($B11&lt;&gt;"",$J11&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E11,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E11,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>500 x 500 px</v>
       </c>
-      <c r="J11" s="109" t="s">
+      <c r="J11" s="78" t="s">
         <v>192</v>
       </c>
       <c r="K11" s="65"/>
@@ -3045,12 +3042,12 @@
         <v>M101</v>
       </c>
     </row>
-    <row r="12" spans="1:16" s="11" customFormat="1" ht="224" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" s="11" customFormat="1" ht="224.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG03</v>
       </c>
-      <c r="B12" s="109" t="s">
+      <c r="B12" s="78" t="s">
         <v>189</v>
       </c>
       <c r="C12" s="20" t="str">
@@ -3079,7 +3076,7 @@
         <f ca="1">IF(OR($B12&lt;&gt;"",$J12&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E12,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E12,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>500 x 500 px</v>
       </c>
-      <c r="J12" s="109" t="s">
+      <c r="J12" s="78" t="s">
         <v>193</v>
       </c>
       <c r="K12" s="64"/>
@@ -3088,12 +3085,12 @@
         <v>Diaporama F1</v>
       </c>
     </row>
-    <row r="13" spans="1:16" s="11" customFormat="1" ht="195" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" s="11" customFormat="1" ht="195" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG04</v>
       </c>
-      <c r="B13" s="109" t="s">
+      <c r="B13" s="78" t="s">
         <v>189</v>
       </c>
       <c r="C13" s="20" t="str">
@@ -3122,7 +3119,7 @@
         <f ca="1">IF(OR($B13&lt;&gt;"",$J13&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E13,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E13,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>500 x 500 px</v>
       </c>
-      <c r="J13" s="109" t="s">
+      <c r="J13" s="78" t="s">
         <v>194</v>
       </c>
       <c r="K13" s="64"/>
@@ -3131,7 +3128,7 @@
         <v>F4</v>
       </c>
     </row>
-    <row r="14" spans="1:16" s="11" customFormat="1" ht="26" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" s="11" customFormat="1" ht="27" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG05</v>
@@ -3165,7 +3162,7 @@
         <f ca="1">IF(OR($B14&lt;&gt;"",$J14&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E14,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E14,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>500 x 500 px</v>
       </c>
-      <c r="J14" s="109" t="s">
+      <c r="J14" s="78" t="s">
         <v>195</v>
       </c>
       <c r="K14" s="64" t="s">
@@ -3176,7 +3173,7 @@
         <v>F6</v>
       </c>
     </row>
-    <row r="15" spans="1:16" s="11" customFormat="1" ht="26" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" s="11" customFormat="1" ht="27" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG06</v>
@@ -3210,7 +3207,7 @@
         <f ca="1">IF(OR($B15&lt;&gt;"",$J15&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E15,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E15,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>500 x 500 px</v>
       </c>
-      <c r="J15" s="109" t="s">
+      <c r="J15" s="78" t="s">
         <v>196</v>
       </c>
       <c r="K15" s="66" t="s">
@@ -3221,7 +3218,7 @@
         <v>F6B</v>
       </c>
     </row>
-    <row r="16" spans="1:16" s="11" customFormat="1" ht="26" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" s="11" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG07</v>
@@ -3255,7 +3252,7 @@
         <f ca="1">IF(OR($B16&lt;&gt;"",$J16&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E16,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E16,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>500 x 500 px</v>
       </c>
-      <c r="J16" s="109" t="s">
+      <c r="J16" s="78" t="s">
         <v>197</v>
       </c>
       <c r="K16" s="68" t="s">
@@ -3266,13 +3263,13 @@
         <v>F7</v>
       </c>
     </row>
-    <row r="17" spans="1:15" s="11" customFormat="1" ht="26" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" s="11" customFormat="1" ht="27" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG08</v>
       </c>
       <c r="B17" s="62">
-        <v>283332293</v>
+        <v>306980027</v>
       </c>
       <c r="C17" s="20" t="str">
         <f t="shared" si="0"/>
@@ -3300,7 +3297,7 @@
         <f ca="1">IF(OR($B17&lt;&gt;"",$J17&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E17,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E17,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>500 x 500 px</v>
       </c>
-      <c r="J17" s="109" t="s">
+      <c r="J17" s="78" t="s">
         <v>198</v>
       </c>
       <c r="K17" s="66" t="s">
@@ -3311,7 +3308,7 @@
         <v>F7B</v>
       </c>
     </row>
-    <row r="18" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3346,7 +3343,7 @@
         <v>F8</v>
       </c>
     </row>
-    <row r="19" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:15" s="11" customFormat="1" ht="14.25" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="str">
         <f t="shared" ref="A19:A50" si="6">IF(OR(B19&lt;&gt;"",J19&lt;&gt;""),CONCATENATE(LEFT(A18,3),IF(MID(A18,4,2)+1&lt;10,CONCATENATE("0",MID(A18,4,2)+1),MID(A18,4,2)+1)),"")</f>
         <v/>
@@ -3381,7 +3378,7 @@
         <v>F10</v>
       </c>
     </row>
-    <row r="20" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3416,7 +3413,7 @@
         <v>F10B</v>
       </c>
     </row>
-    <row r="21" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3451,7 +3448,7 @@
         <v>F11</v>
       </c>
     </row>
-    <row r="22" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3486,7 +3483,7 @@
         <v>F12</v>
       </c>
     </row>
-    <row r="23" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3521,7 +3518,7 @@
         <v>F13</v>
       </c>
     </row>
-    <row r="24" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3556,7 +3553,7 @@
         <v>F13B</v>
       </c>
     </row>
-    <row r="25" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3587,7 +3584,7 @@
       <c r="J25" s="63"/>
       <c r="K25" s="64"/>
     </row>
-    <row r="26" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3618,7 +3615,7 @@
       <c r="J26" s="63"/>
       <c r="K26" s="64"/>
     </row>
-    <row r="27" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3650,7 +3647,7 @@
       <c r="K27" s="64"/>
       <c r="O27" s="2"/>
     </row>
-    <row r="28" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3681,7 +3678,7 @@
       <c r="J28" s="64"/>
       <c r="K28" s="64"/>
     </row>
-    <row r="29" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3712,7 +3709,7 @@
       <c r="J29" s="64"/>
       <c r="K29" s="64"/>
     </row>
-    <row r="30" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3743,7 +3740,7 @@
       <c r="J30" s="64"/>
       <c r="K30" s="64"/>
     </row>
-    <row r="31" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3774,7 +3771,7 @@
       <c r="J31" s="64"/>
       <c r="K31" s="64"/>
     </row>
-    <row r="32" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3805,7 +3802,7 @@
       <c r="J32" s="64"/>
       <c r="K32" s="64"/>
     </row>
-    <row r="33" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3836,7 +3833,7 @@
       <c r="J33" s="64"/>
       <c r="K33" s="64"/>
     </row>
-    <row r="34" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3868,7 +3865,7 @@
       <c r="K34" s="64"/>
       <c r="O34" s="2"/>
     </row>
-    <row r="35" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3900,7 +3897,7 @@
       <c r="K35" s="65"/>
       <c r="O35" s="2"/>
     </row>
-    <row r="36" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3932,7 +3929,7 @@
       <c r="K36" s="65"/>
       <c r="O36" s="2"/>
     </row>
-    <row r="37" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3963,7 +3960,7 @@
       <c r="J37" s="70"/>
       <c r="K37" s="65"/>
     </row>
-    <row r="38" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3994,7 +3991,7 @@
       <c r="J38" s="71"/>
       <c r="K38" s="65"/>
     </row>
-    <row r="39" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4025,7 +4022,7 @@
       <c r="J39" s="63"/>
       <c r="K39" s="65"/>
     </row>
-    <row r="40" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4056,7 +4053,7 @@
       <c r="J40" s="63"/>
       <c r="K40" s="65"/>
     </row>
-    <row r="41" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4087,7 +4084,7 @@
       <c r="J41" s="63"/>
       <c r="K41" s="65"/>
     </row>
-    <row r="42" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4118,7 +4115,7 @@
       <c r="J42" s="63"/>
       <c r="K42" s="65"/>
     </row>
-    <row r="43" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4149,7 +4146,7 @@
       <c r="J43" s="63"/>
       <c r="K43" s="65"/>
     </row>
-    <row r="44" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4180,7 +4177,7 @@
       <c r="J44" s="63"/>
       <c r="K44" s="65"/>
     </row>
-    <row r="45" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4211,7 +4208,7 @@
       <c r="J45" s="63"/>
       <c r="K45" s="65"/>
     </row>
-    <row r="46" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4242,7 +4239,7 @@
       <c r="J46" s="63"/>
       <c r="K46" s="65"/>
     </row>
-    <row r="47" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4273,7 +4270,7 @@
       <c r="J47" s="63"/>
       <c r="K47" s="65"/>
     </row>
-    <row r="48" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4304,7 +4301,7 @@
       <c r="J48" s="63"/>
       <c r="K48" s="65"/>
     </row>
-    <row r="49" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4335,7 +4332,7 @@
       <c r="J49" s="63"/>
       <c r="K49" s="65"/>
     </row>
-    <row r="50" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4366,7 +4363,7 @@
       <c r="J50" s="63"/>
       <c r="K50" s="65"/>
     </row>
-    <row r="51" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="12" t="str">
         <f t="shared" ref="A51:A82" si="8">IF(OR(B51&lt;&gt;"",J51&lt;&gt;""),CONCATENATE(LEFT(A50,3),IF(MID(A50,4,2)+1&lt;10,CONCATENATE("0",MID(A50,4,2)+1),MID(A50,4,2)+1)),"")</f>
         <v/>
@@ -4397,7 +4394,7 @@
       <c r="J51" s="63"/>
       <c r="K51" s="65"/>
     </row>
-    <row r="52" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4428,7 +4425,7 @@
       <c r="J52" s="63"/>
       <c r="K52" s="65"/>
     </row>
-    <row r="53" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4459,7 +4456,7 @@
       <c r="J53" s="63"/>
       <c r="K53" s="65"/>
     </row>
-    <row r="54" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4490,7 +4487,7 @@
       <c r="J54" s="63"/>
       <c r="K54" s="65"/>
     </row>
-    <row r="55" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4521,7 +4518,7 @@
       <c r="J55" s="63"/>
       <c r="K55" s="65"/>
     </row>
-    <row r="56" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4552,7 +4549,7 @@
       <c r="J56" s="63"/>
       <c r="K56" s="65"/>
     </row>
-    <row r="57" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4583,7 +4580,7 @@
       <c r="J57" s="63"/>
       <c r="K57" s="65"/>
     </row>
-    <row r="58" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4614,7 +4611,7 @@
       <c r="J58" s="63"/>
       <c r="K58" s="65"/>
     </row>
-    <row r="59" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4645,7 +4642,7 @@
       <c r="J59" s="63"/>
       <c r="K59" s="65"/>
     </row>
-    <row r="60" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4676,7 +4673,7 @@
       <c r="J60" s="63"/>
       <c r="K60" s="65"/>
     </row>
-    <row r="61" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4707,7 +4704,7 @@
       <c r="J61" s="63"/>
       <c r="K61" s="65"/>
     </row>
-    <row r="62" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4738,7 +4735,7 @@
       <c r="J62" s="63"/>
       <c r="K62" s="65"/>
     </row>
-    <row r="63" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4769,7 +4766,7 @@
       <c r="J63" s="63"/>
       <c r="K63" s="65"/>
     </row>
-    <row r="64" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4800,7 +4797,7 @@
       <c r="J64" s="63"/>
       <c r="K64" s="65"/>
     </row>
-    <row r="65" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4831,7 +4828,7 @@
       <c r="J65" s="63"/>
       <c r="K65" s="65"/>
     </row>
-    <row r="66" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4862,7 +4859,7 @@
       <c r="J66" s="63"/>
       <c r="K66" s="65"/>
     </row>
-    <row r="67" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4893,7 +4890,7 @@
       <c r="J67" s="63"/>
       <c r="K67" s="65"/>
     </row>
-    <row r="68" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4924,7 +4921,7 @@
       <c r="J68" s="63"/>
       <c r="K68" s="65"/>
     </row>
-    <row r="69" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4955,7 +4952,7 @@
       <c r="J69" s="63"/>
       <c r="K69" s="65"/>
     </row>
-    <row r="70" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4986,7 +4983,7 @@
       <c r="J70" s="63"/>
       <c r="K70" s="65"/>
     </row>
-    <row r="71" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5017,7 +5014,7 @@
       <c r="J71" s="63"/>
       <c r="K71" s="65"/>
     </row>
-    <row r="72" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5048,7 +5045,7 @@
       <c r="J72" s="63"/>
       <c r="K72" s="65"/>
     </row>
-    <row r="73" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5079,7 +5076,7 @@
       <c r="J73" s="63"/>
       <c r="K73" s="65"/>
     </row>
-    <row r="74" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5110,7 +5107,7 @@
       <c r="J74" s="63"/>
       <c r="K74" s="65"/>
     </row>
-    <row r="75" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5141,7 +5138,7 @@
       <c r="J75" s="63"/>
       <c r="K75" s="65"/>
     </row>
-    <row r="76" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5172,7 +5169,7 @@
       <c r="J76" s="63"/>
       <c r="K76" s="65"/>
     </row>
-    <row r="77" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5203,7 +5200,7 @@
       <c r="J77" s="63"/>
       <c r="K77" s="65"/>
     </row>
-    <row r="78" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5234,7 +5231,7 @@
       <c r="J78" s="63"/>
       <c r="K78" s="65"/>
     </row>
-    <row r="79" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5265,7 +5262,7 @@
       <c r="J79" s="63"/>
       <c r="K79" s="65"/>
     </row>
-    <row r="80" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5296,7 +5293,7 @@
       <c r="J80" s="63"/>
       <c r="K80" s="65"/>
     </row>
-    <row r="81" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5327,7 +5324,7 @@
       <c r="J81" s="63"/>
       <c r="K81" s="65"/>
     </row>
-    <row r="82" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5358,7 +5355,7 @@
       <c r="J82" s="63"/>
       <c r="K82" s="65"/>
     </row>
-    <row r="83" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="12" t="str">
         <f t="shared" ref="A83:A108" si="12">IF(OR(B83&lt;&gt;"",J83&lt;&gt;""),CONCATENATE(LEFT(A82,3),IF(MID(A82,4,2)+1&lt;10,CONCATENATE("0",MID(A82,4,2)+1),MID(A82,4,2)+1)),"")</f>
         <v/>
@@ -5389,7 +5386,7 @@
       <c r="J83" s="63"/>
       <c r="K83" s="65"/>
     </row>
-    <row r="84" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5420,7 +5417,7 @@
       <c r="J84" s="63"/>
       <c r="K84" s="65"/>
     </row>
-    <row r="85" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5451,7 +5448,7 @@
       <c r="J85" s="63"/>
       <c r="K85" s="65"/>
     </row>
-    <row r="86" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5482,7 +5479,7 @@
       <c r="J86" s="63"/>
       <c r="K86" s="65"/>
     </row>
-    <row r="87" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5513,7 +5510,7 @@
       <c r="J87" s="63"/>
       <c r="K87" s="65"/>
     </row>
-    <row r="88" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5544,7 +5541,7 @@
       <c r="J88" s="63"/>
       <c r="K88" s="65"/>
     </row>
-    <row r="89" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5575,7 +5572,7 @@
       <c r="J89" s="63"/>
       <c r="K89" s="65"/>
     </row>
-    <row r="90" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5606,7 +5603,7 @@
       <c r="J90" s="63"/>
       <c r="K90" s="65"/>
     </row>
-    <row r="91" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5637,7 +5634,7 @@
       <c r="J91" s="63"/>
       <c r="K91" s="65"/>
     </row>
-    <row r="92" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5668,7 +5665,7 @@
       <c r="J92" s="63"/>
       <c r="K92" s="65"/>
     </row>
-    <row r="93" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5699,7 +5696,7 @@
       <c r="J93" s="63"/>
       <c r="K93" s="65"/>
     </row>
-    <row r="94" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5730,7 +5727,7 @@
       <c r="J94" s="63"/>
       <c r="K94" s="65"/>
     </row>
-    <row r="95" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5761,7 +5758,7 @@
       <c r="J95" s="63"/>
       <c r="K95" s="65"/>
     </row>
-    <row r="96" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5792,7 +5789,7 @@
       <c r="J96" s="63"/>
       <c r="K96" s="65"/>
     </row>
-    <row r="97" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5823,7 +5820,7 @@
       <c r="J97" s="63"/>
       <c r="K97" s="65"/>
     </row>
-    <row r="98" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5854,7 +5851,7 @@
       <c r="J98" s="63"/>
       <c r="K98" s="65"/>
     </row>
-    <row r="99" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5885,7 +5882,7 @@
       <c r="J99" s="63"/>
       <c r="K99" s="65"/>
     </row>
-    <row r="100" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5916,7 +5913,7 @@
       <c r="J100" s="63"/>
       <c r="K100" s="65"/>
     </row>
-    <row r="101" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5947,7 +5944,7 @@
       <c r="J101" s="63"/>
       <c r="K101" s="65"/>
     </row>
-    <row r="102" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5978,7 +5975,7 @@
       <c r="J102" s="63"/>
       <c r="K102" s="65"/>
     </row>
-    <row r="103" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -6009,7 +6006,7 @@
       <c r="J103" s="63"/>
       <c r="K103" s="65"/>
     </row>
-    <row r="104" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -6040,7 +6037,7 @@
       <c r="J104" s="63"/>
       <c r="K104" s="65"/>
     </row>
-    <row r="105" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -6071,7 +6068,7 @@
       <c r="J105" s="63"/>
       <c r="K105" s="65"/>
     </row>
-    <row r="106" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -6102,7 +6099,7 @@
       <c r="J106" s="63"/>
       <c r="K106" s="65"/>
     </row>
-    <row r="107" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -6133,7 +6130,7 @@
       <c r="J107" s="63"/>
       <c r="K107" s="65"/>
     </row>
-    <row r="108" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -6212,56 +6209,56 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Hoja2" enableFormatConditionsCalculation="0"/>
+  <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="72.1640625" style="22" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="22"/>
-    <col min="3" max="3" width="13.83203125" style="22" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" style="22" customWidth="1"/>
-    <col min="5" max="7" width="10.83203125" style="22"/>
+    <col min="1" max="1" width="72.125" style="22" customWidth="1"/>
+    <col min="2" max="2" width="10.875" style="22"/>
+    <col min="3" max="3" width="13.875" style="22" customWidth="1"/>
+    <col min="4" max="4" width="11.375" style="22" customWidth="1"/>
+    <col min="5" max="7" width="10.875" style="22"/>
     <col min="8" max="11" width="11" style="22" hidden="1" customWidth="1"/>
-    <col min="12" max="16384" width="10.83203125" style="22"/>
+    <col min="12" max="16384" width="10.875" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="93" t="s">
+    <row r="1" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="94" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="95"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="95"/>
+      <c r="F1" s="96"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
         <v>42</v>
       </c>
       <c r="B2" s="31"/>
-      <c r="C2" s="96" t="s">
+      <c r="C2" s="97" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="97"/>
-      <c r="E2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="99"/>
       <c r="F2" s="32"/>
     </row>
-    <row r="3" spans="1:11" ht="64" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="63" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
         <v>43</v>
       </c>
       <c r="B3" s="31"/>
-      <c r="C3" s="102" t="s">
+      <c r="C3" s="103" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="103"/>
-      <c r="E3" s="104"/>
+      <c r="D3" s="104"/>
+      <c r="E3" s="105"/>
       <c r="F3" s="32"/>
       <c r="H3" s="22" t="s">
         <v>18</v>
@@ -6276,7 +6273,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="30" t="s">
         <v>44</v>
       </c>
@@ -6304,7 +6301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="81" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="33" t="s">
         <v>45</v>
       </c>
@@ -6312,11 +6309,11 @@
       <c r="C5" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="105" t="str">
+      <c r="D5" s="106" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_CO")</f>
         <v>LE_07_04_CO</v>
       </c>
-      <c r="E5" s="106"/>
+      <c r="E5" s="107"/>
       <c r="F5" s="32"/>
       <c r="H5" s="22" t="s">
         <v>22</v>
@@ -6331,7 +6328,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="30" t="s">
         <v>10</v>
       </c>
@@ -6353,7 +6350,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="33" t="s">
         <v>11</v>
       </c>
@@ -6361,12 +6358,12 @@
       <c r="C7" s="59" t="s">
         <v>119</v>
       </c>
-      <c r="D7" s="91" t="str">
+      <c r="D7" s="92" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D5,".xls")</f>
         <v>SolicitudGrafica_LE_07_04_CO.xls</v>
       </c>
-      <c r="E7" s="91"/>
-      <c r="F7" s="92"/>
+      <c r="E7" s="92"/>
+      <c r="F7" s="93"/>
       <c r="H7" s="22" t="s">
         <v>24</v>
       </c>
@@ -6380,7 +6377,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
         <v>53</v>
       </c>
@@ -6399,7 +6396,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
         <v>12</v>
       </c>
@@ -6418,7 +6415,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="34" t="s">
         <v>36</v>
       </c>
@@ -6437,7 +6434,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I11" s="22" t="s">
         <v>32</v>
       </c>
@@ -6448,7 +6445,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I12" s="22" t="s">
         <v>37</v>
       </c>
@@ -6459,15 +6456,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="93" t="s">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="94" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="94"/>
-      <c r="C13" s="94"/>
-      <c r="D13" s="94"/>
-      <c r="E13" s="94"/>
-      <c r="F13" s="95"/>
+      <c r="B13" s="95"/>
+      <c r="C13" s="95"/>
+      <c r="D13" s="95"/>
+      <c r="E13" s="95"/>
+      <c r="F13" s="96"/>
       <c r="I13" s="22" t="s">
         <v>33</v>
       </c>
@@ -6478,7 +6475,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="33"/>
       <c r="B14" s="31"/>
       <c r="C14" s="31"/>
@@ -6495,17 +6492,17 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="30" t="s">
         <v>46</v>
       </c>
       <c r="B15" s="31"/>
-      <c r="C15" s="96" t="s">
+      <c r="C15" s="97" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="97"/>
-      <c r="E15" s="97"/>
-      <c r="F15" s="98"/>
+      <c r="D15" s="98"/>
+      <c r="E15" s="98"/>
+      <c r="F15" s="99"/>
       <c r="J15" s="22">
         <v>12</v>
       </c>
@@ -6513,7 +6510,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="67" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="66.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="33" t="s">
         <v>47</v>
       </c>
@@ -6537,7 +6534,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="30" t="s">
         <v>44</v>
       </c>
@@ -6545,12 +6542,12 @@
       <c r="C17" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="99" t="str">
+      <c r="D17" s="100" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_",K45)</f>
         <v>LE_07_04_REC10</v>
       </c>
-      <c r="E17" s="100"/>
-      <c r="F17" s="101"/>
+      <c r="E17" s="101"/>
+      <c r="F17" s="102"/>
       <c r="J17" s="22">
         <v>14</v>
       </c>
@@ -6558,7 +6555,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="81" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="33" t="s">
         <v>48</v>
       </c>
@@ -6566,12 +6563,12 @@
       <c r="C18" s="59" t="s">
         <v>120</v>
       </c>
-      <c r="D18" s="91" t="str">
+      <c r="D18" s="92" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D17,".xls")</f>
         <v>SolicitudGrafica_LE_07_04_REC10.xls</v>
       </c>
-      <c r="E18" s="91"/>
-      <c r="F18" s="92"/>
+      <c r="E18" s="92"/>
+      <c r="F18" s="93"/>
       <c r="J18" s="22">
         <v>15</v>
       </c>
@@ -6579,7 +6576,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="30" t="s">
         <v>10</v>
       </c>
@@ -6598,7 +6595,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="65" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="34" t="s">
         <v>51</v>
       </c>
@@ -6620,7 +6617,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H21" s="22" t="str">
         <f>IF(INDEX(H4:H7,H20)=H4,"MA",IF(INDEX(H4:H7,H20)=H5,"CN",IF(INDEX(H4:H7,H20)=H6,"CS",IF(INDEX(H4:H7,H20)=H7,"LE"))))</f>
         <v>LE</v>
@@ -6637,122 +6634,122 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K22" s="22">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K23" s="22">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K24" s="22">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K25" s="22">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K26" s="22">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K27" s="22">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K28" s="22">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K29" s="22">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K30" s="22">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K31" s="22">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K32" s="22">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K33" s="22">
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K34" s="22">
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K35" s="22">
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K36" s="22">
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K37" s="22">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K38" s="22">
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K39" s="22">
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K40" s="22">
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K41" s="22">
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K42" s="22">
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K43" s="22">
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K44" s="22">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K45" s="22" t="str">
         <f>CONCATENATE("REC",K44,0)</f>
         <v>REC10</v>
@@ -6786,19 +6783,18 @@
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>482600</xdr:rowOff>
+                    <xdr:rowOff>485775</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>1016000</xdr:colOff>
+                    <xdr:colOff>1019175</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>711200</xdr:rowOff>
+                    <xdr:rowOff>714375</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
-          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
@@ -6807,21 +6803,20 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>1016000</xdr:colOff>
+                    <xdr:colOff>1019175</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>482600</xdr:rowOff>
+                    <xdr:rowOff>485775</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
                     <xdr:colOff>838200</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>711200</xdr:rowOff>
+                    <xdr:rowOff>714375</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
-          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
@@ -6832,19 +6827,18 @@
                     <xdr:col>4</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>482600</xdr:rowOff>
+                    <xdr:rowOff>485775</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
                     <xdr:colOff>838200</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>711200</xdr:rowOff>
+                    <xdr:rowOff>714375</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
-          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
@@ -6855,19 +6849,18 @@
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>482600</xdr:rowOff>
+                    <xdr:rowOff>485775</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>838200</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>711200</xdr:rowOff>
+                    <xdr:rowOff>714375</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
-          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
@@ -6876,13 +6869,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>25400</xdr:colOff>
+                    <xdr:colOff>28575</xdr:colOff>
                     <xdr:row>4</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>1041400</xdr:colOff>
+                    <xdr:colOff>1038225</xdr:colOff>
                     <xdr:row>4</xdr:row>
                     <xdr:rowOff>228600</xdr:rowOff>
                   </to>
@@ -6890,7 +6883,6 @@
               </controlPr>
             </control>
           </mc:Choice>
-          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
@@ -6899,13 +6891,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>1054100</xdr:colOff>
+                    <xdr:colOff>1057275</xdr:colOff>
                     <xdr:row>4</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>863600</xdr:colOff>
+                    <xdr:colOff>866775</xdr:colOff>
                     <xdr:row>4</xdr:row>
                     <xdr:rowOff>228600</xdr:rowOff>
                   </to>
@@ -6913,7 +6905,6 @@
               </controlPr>
             </control>
           </mc:Choice>
-          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
@@ -6922,7 +6913,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>12700</xdr:colOff>
+                    <xdr:colOff>9525</xdr:colOff>
                     <xdr:row>4</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
@@ -6936,11 +6927,9 @@
               </controlPr>
             </control>
           </mc:Choice>
-          <mc:Fallback/>
         </mc:AlternateContent>
       </controls>
     </mc:Choice>
-    <mc:Fallback/>
   </mc:AlternateContent>
 </worksheet>
 </file>
@@ -6954,56 +6943,56 @@
       <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" style="22" customWidth="1"/>
-    <col min="2" max="2" width="24.1640625" style="22" customWidth="1"/>
+    <col min="2" max="2" width="24.125" style="22" customWidth="1"/>
     <col min="3" max="3" width="17" style="22" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="22" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" style="22" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" style="22" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" style="22" customWidth="1"/>
+    <col min="4" max="4" width="12.625" style="22" customWidth="1"/>
+    <col min="5" max="5" width="6.875" style="22" customWidth="1"/>
+    <col min="6" max="6" width="12.875" style="22" customWidth="1"/>
+    <col min="7" max="7" width="12.625" style="22" customWidth="1"/>
     <col min="8" max="8" width="24.5" style="22" customWidth="1"/>
-    <col min="9" max="9" width="27.1640625" style="22" customWidth="1"/>
+    <col min="9" max="9" width="27.125" style="22" customWidth="1"/>
     <col min="10" max="10" width="44.5" style="22" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="22"/>
+    <col min="11" max="16384" width="10.875" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="108" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="109" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="108" t="s">
+      <c r="B1" s="109" t="s">
         <v>149</v>
       </c>
-      <c r="C1" s="108" t="s">
+      <c r="C1" s="109" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="108" t="s">
+      <c r="D1" s="109" t="s">
         <v>64</v>
       </c>
-      <c r="E1" s="108" t="s">
+      <c r="E1" s="109" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="108" t="s">
+      <c r="F1" s="109" t="s">
         <v>65</v>
       </c>
-      <c r="G1" s="108" t="s">
+      <c r="G1" s="109" t="s">
         <v>66</v>
       </c>
-      <c r="H1" s="107" t="s">
+      <c r="H1" s="108" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="107"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="108"/>
-      <c r="B2" s="108"/>
-      <c r="C2" s="108"/>
-      <c r="D2" s="108"/>
-      <c r="E2" s="108"/>
-      <c r="F2" s="108"/>
-      <c r="G2" s="108"/>
+      <c r="I1" s="108"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="109"/>
+      <c r="B2" s="109"/>
+      <c r="C2" s="109"/>
+      <c r="D2" s="109"/>
+      <c r="E2" s="109"/>
+      <c r="F2" s="109"/>
+      <c r="G2" s="109"/>
       <c r="H2" s="39" t="s">
         <v>65</v>
       </c>
@@ -7011,7 +7000,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:10" s="41" customFormat="1" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
         <v>69</v>
       </c>
@@ -7036,7 +7025,7 @@
       </c>
       <c r="I3" s="40"/>
     </row>
-    <row r="4" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:10" s="41" customFormat="1" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="42" t="s">
         <v>57</v>
       </c>
@@ -7065,7 +7054,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:10" s="41" customFormat="1" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="43" t="s">
         <v>77</v>
       </c>
@@ -7094,7 +7083,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" s="41" customFormat="1" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="42" t="s">
         <v>58</v>
       </c>
@@ -7123,7 +7112,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" s="41" customFormat="1" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="42" t="s">
         <v>58</v>
       </c>
@@ -7148,7 +7137,7 @@
       </c>
       <c r="I7" s="42"/>
     </row>
-    <row r="8" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:10" s="41" customFormat="1" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="42" t="s">
         <v>80</v>
       </c>
@@ -7177,7 +7166,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:10" s="41" customFormat="1" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="42" t="s">
         <v>82</v>
       </c>
@@ -7206,7 +7195,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:10" s="41" customFormat="1" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="42" t="s">
         <v>84</v>
       </c>
@@ -7235,7 +7224,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" s="41" customFormat="1" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="42" t="s">
         <v>86</v>
       </c>
@@ -7260,7 +7249,7 @@
       </c>
       <c r="I11" s="42"/>
     </row>
-    <row r="12" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" s="41" customFormat="1" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="42" t="s">
         <v>89</v>
       </c>
@@ -7289,7 +7278,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:10" s="41" customFormat="1" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="42" t="s">
         <v>91</v>
       </c>
@@ -7318,7 +7307,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="44" t="s">
         <v>94</v>
       </c>
@@ -7341,7 +7330,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="77" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" s="77" customFormat="1" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="75" t="s">
         <v>96</v>
       </c>
@@ -7367,7 +7356,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="46" t="s">
         <v>100</v>
       </c>
@@ -7395,7 +7384,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="42" t="s">
         <v>103</v>
       </c>
@@ -7423,7 +7412,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:10" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="42" t="s">
         <v>184</v>
       </c>
@@ -7449,7 +7438,7 @@
       <c r="I18" s="44"/>
       <c r="J18" s="49"/>
     </row>
-    <row r="19" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:10" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="42" t="s">
         <v>137</v>
       </c>
@@ -7473,7 +7462,7 @@
       <c r="I19" s="44"/>
       <c r="J19" s="49"/>
     </row>
-    <row r="20" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:10" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="42" t="s">
         <v>137</v>
       </c>
@@ -7497,7 +7486,7 @@
       <c r="I20" s="44"/>
       <c r="J20" s="49"/>
     </row>
-    <row r="21" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:10" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="42" t="s">
         <v>137</v>
       </c>
@@ -7521,7 +7510,7 @@
       <c r="I21" s="72"/>
       <c r="J21" s="49"/>
     </row>
-    <row r="22" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="44" t="s">
         <v>132</v>
       </c>
@@ -7545,7 +7534,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="42" t="s">
         <v>132</v>
       </c>
@@ -7574,7 +7563,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="42" t="s">
         <v>134</v>
       </c>
@@ -7597,7 +7586,7 @@
       <c r="H24" s="44"/>
       <c r="I24" s="72"/>
     </row>
-    <row r="25" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="42" t="s">
         <v>135</v>
       </c>
@@ -7621,7 +7610,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="42" t="s">
         <v>135</v>
       </c>
@@ -7650,7 +7639,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="42" t="s">
         <v>138</v>
       </c>
@@ -7674,7 +7663,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="42" t="s">
         <v>138</v>
       </c>
@@ -7698,7 +7687,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="42" t="s">
         <v>138</v>
       </c>
@@ -7727,7 +7716,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="42" t="s">
         <v>139</v>
       </c>
@@ -7750,7 +7739,7 @@
       <c r="H30" s="44"/>
       <c r="I30" s="44"/>
     </row>
-    <row r="31" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="42" t="s">
         <v>140</v>
       </c>
@@ -7767,7 +7756,7 @@
       <c r="H31" s="44"/>
       <c r="I31" s="44"/>
     </row>
-    <row r="32" spans="1:10" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="42" t="s">
         <v>141</v>
       </c>
@@ -7782,7 +7771,7 @@
       <c r="H32" s="44"/>
       <c r="I32" s="44"/>
     </row>
-    <row r="33" spans="1:9" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="42" t="s">
         <v>136</v>
       </c>
@@ -7803,7 +7792,7 @@
       <c r="H33" s="44"/>
       <c r="I33" s="44"/>
     </row>
-    <row r="34" spans="1:9" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="42" t="s">
         <v>142</v>
       </c>
@@ -7820,7 +7809,7 @@
       <c r="H34" s="44"/>
       <c r="I34" s="44"/>
     </row>
-    <row r="35" spans="1:9" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="42" t="s">
         <v>95</v>
       </c>
@@ -7849,7 +7838,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="42" t="s">
         <v>95</v>
       </c>
@@ -7878,7 +7867,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="42" t="s">
         <v>143</v>
       </c>
@@ -7901,7 +7890,7 @@
       <c r="H37" s="44"/>
       <c r="I37" s="44"/>
     </row>
-    <row r="38" spans="1:9" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="42" t="s">
         <v>143</v>
       </c>
@@ -7924,13 +7913,13 @@
       <c r="H38" s="44"/>
       <c r="I38" s="44"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="50" t="s">
         <v>107</v>
       </c>
       <c r="B40" s="50"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="51" t="s">
         <v>108</v>
       </c>
@@ -7944,7 +7933,7 @@
       <c r="E41" s="52"/>
       <c r="F41" s="52"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="54" t="s">
         <v>109</v>
       </c>
@@ -7958,7 +7947,7 @@
       <c r="E42" s="55"/>
       <c r="F42" s="55"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="54" t="s">
         <v>110</v>
       </c>
@@ -7972,7 +7961,7 @@
       <c r="E43" s="55"/>
       <c r="F43" s="55"/>
     </row>
-    <row r="44" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A44" s="54" t="s">
         <v>111</v>
       </c>
@@ -7986,7 +7975,7 @@
       <c r="E44" s="55"/>
       <c r="F44" s="55"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="54" t="s">
         <v>112</v>
       </c>
@@ -8000,7 +7989,7 @@
       <c r="E45" s="55"/>
       <c r="F45" s="55"/>
     </row>
-    <row r="46" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A46" s="54" t="s">
         <v>162</v>
       </c>

</xml_diff>